<commit_message>
feat: teste de mesa bubble sort  array 2
</commit_message>
<xml_diff>
--- a/testes_de_mesa/Sorts.xlsx
+++ b/testes_de_mesa/Sorts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\OneDrive\Área de Trabalho\Projeto_Java\Exercícios_ED\Sorts\testes_de_mesa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B055B6D3-9A25-4F79-BA2B-22DBA6AD490B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B6964-5C5D-4A2E-B190-3485625759C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF2CA25F-5BEF-4103-8C21-7B5DA73C0FC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AF2CA25F-5BEF-4103-8C21-7B5DA73C0FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="MergeSort1" sheetId="1" r:id="rId1"/>
+    <sheet name="MergeSort2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Metade</t>
   </si>
@@ -51,6 +52,12 @@
   </si>
   <si>
     <t>Metade D</t>
+  </si>
+  <si>
+    <t>Rodada 1</t>
+  </si>
+  <si>
+    <t>Rodada 2</t>
   </si>
 </sst>
 </file>
@@ -107,11 +114,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,6 +139,529 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Retângulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFAD7D13-CBCC-B0C8-387F-CA72779D0466}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7229475" y="2638425"/>
+          <a:ext cx="2447925" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Aqui</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> é o Merge Sort indo até o ponto de parada.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0358F8C3-9F4C-4130-864F-351C18ECC3C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7096125" y="2714625"/>
+          <a:ext cx="2447925" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Aqui</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> é o Merge Sort ordenando seus valores.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>132960</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>98040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>217080</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57120</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Tinta 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067978BD-CD39-9364-63BF-A3920E6A5CA5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1352160" y="2003040"/>
+            <a:ext cx="693720" cy="721080"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Tinta 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067978BD-CD39-9364-63BF-A3920E6A5CA5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1343520" y="1994400"/>
+              <a:ext cx="711360" cy="738720"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152160</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257880</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>37860</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="10" name="Tinta 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB72F73-7B34-F45D-F7AF-6939C7F79AED}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4419360" y="1504800"/>
+            <a:ext cx="715320" cy="628560"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="10" name="Tinta 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB72F73-7B34-F45D-F7AF-6939C7F79AED}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4410360" y="1495800"/>
+              <a:ext cx="732960" cy="646200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>75720</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>132240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19020</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="13" name="Tinta 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5122B0AA-90D5-EE28-28EB-99EE0D236FD3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4952520" y="894240"/>
+            <a:ext cx="133920" cy="458280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Tinta 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5122B0AA-90D5-EE28-28EB-99EE0D236FD3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4943880" y="885240"/>
+              <a:ext cx="151560" cy="475920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66360</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>188760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>163800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>240</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="16" name="Tinta 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBDBDCC9-0A9C-4D67-73BC-751F6795D5C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6771960" y="2093760"/>
+            <a:ext cx="707040" cy="573480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="16" name="Tinta 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBDBDCC9-0A9C-4D67-73BC-751F6795D5C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6763320" y="2084760"/>
+              <a:ext cx="724680" cy="591120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-27T02:09:52.237"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2003 24575,'22'-3'0,"1"-1"0,-1-1 0,0-1 0,0-1 0,-1-1 0,34-17 0,-41 18 0,476-253 0,-347 171 0,-5-6 0,138-124 0,-255 199 0,0-2 0,-2 0 0,0 0 0,25-41 0,49-107 0,-59 102 0,45-63 0,-61 104 0,-1 0 0,0 0 0,-3-2 0,0 0 0,-1 0 0,-2-1 0,-2-1 0,0 0 0,-2 0 0,-2-1 0,0 0 0,-1-63 0,-2 35 0,-1 36 0,0 1 0,-2-1 0,0 1 0,-8-39 0,7 55 0,-1 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,0 1 0,-1-1 0,-6-5 0,-6-9 0,17 19 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,2 1 0,31 3 0,-31-4 0,184 11-1365,-156-10-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="958.43">1641 18 24575,'-5'5'0,"-1"5"0,1 6 0,0 10 0,-2-1 0,-6 1 0,0 0 0,2 1 0,4-6-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-27T02:13:23.368"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1746 24575,'-1'-13'0,"2"1"0,-1 0 0,2-1 0,-1 1 0,2 0 0,0 0 0,0 0 0,1 0 0,1 0 0,0 1 0,0 0 0,1 0 0,0 0 0,1 1 0,1 0 0,-1 0 0,2 1 0,-1 0 0,15-12 0,256-205 0,-175 137 0,-67 60 0,73-40 0,19-15 0,-117 75 0,1 1 0,0 1 0,0 0 0,1 1 0,0 0 0,0 1 0,0 1 0,1 0 0,0 1 0,25-2 0,15 1 0,89 7 0,-40 1 0,-46-6 0,-1-2 0,0-2 0,0-3 0,-1-3 0,0-2 0,-1-2 0,76-34 0,-118 43 0,0 0 0,0 0 0,-1-1 0,0-1 0,0 0 0,-1-1 0,0 0 0,-1 0 0,0-1 0,-1-1 0,0 1 0,-1-2 0,0 1 0,6-15 0,-5 7 0,-1-1 0,0 0 0,-2 0 0,-1-1 0,0 0 0,-2 0 0,0 0 0,-1-34 0,-2 53 0,0-21 0,0 0 0,-2-1 0,-8-42 0,8 58 0,-1 1 0,0 1 0,0-1 0,-1 0 0,0 1 0,0 0 0,0 0 0,-1 0 0,0 0 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,-8-5 0,-15-8 0,0 1 0,-1 2 0,0 1 0,-1 1 0,-1 2 0,0 1 0,-55-10 0,85 20-4,0 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-2-3 1,2 3 13,1 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,1-1-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 1-1,1-2 1,1-1-123,1 0 0,-1 0-1,1 0 1,0 0 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,0 2-1,1-1 1,7-3 0,9 0-6712</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1531.32">1562 26 24575,'-5'9'0,"-1"8"0,5 0 0,2 2 0,2 3 0,-1 2 0,0 1 0,0 1 0,-1-4-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2863.28">1562 26 24575,'4'0'0,"6"0"0,7 0 0,3 0 0,13-5 0,1 0-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-27T02:14:24.723"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1273 24575,'1'0'0,"1"-1"0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1-2 0,21-44 0,-10 18 0,27-45 0,-2-2 0,32-98 0,-45 112 0,-15 42 0,-2 1 0,0-2 0,-2 1 0,0-1 0,-1 0 0,3-32 0,-9-153 0,-1 82 0,2 112 0,-1 0 0,0 0 0,-1 0 0,-1 0 0,0 1 0,-1-1 0,-10-22 0,2 10 0,-2 1 0,-26-35 0,40 58 0,-1 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,3 1 0,63 10 0,-25 2-1365,-4-2-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1662.27">160 82 24575,'0'5'0,"0"5"0,0 6 0,0 5 0,0 3 0,0 2 0,0 1 0,0-4-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-02-27T02:16:23.835"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1592 24575,'128'-6'0,"0"-6"0,205-46 0,-171 30 0,121-28 0,-239 44 0,-1-2 0,0-1 0,-1-3 0,53-29 0,-74 32 0,-1-1 0,-1-1 0,0 0 0,-2-1 0,0-1 0,19-27 0,17-18 0,-9 18 0,1 3 0,3 1 0,80-53 0,-110 83 0,-1-1 0,-1 0 0,0-1 0,-1-1 0,-1-1 0,0 0 0,17-26 0,-23 29 0,-1 0 0,-1-1 0,0 1 0,0-1 0,-2-1 0,0 1 0,0-1 0,-1 0 0,-1 0 0,-1 0 0,0-17 0,-1-15 0,1 11 0,-2-1 0,-7-52 0,6 78 0,-1 0 0,0 0 0,0 1 0,-1-1 0,0 1 0,-1 0 0,0 0 0,-1 1 0,0-1 0,0 1 0,-1 1 0,-11-13 0,-24-12 0,-22-21 0,62 51 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1-6 0,0 8 5,1-1-1,0 1 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 1 0,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0 0 0,1 0 1,-1 1-1,0-1 1,1 0-1,4 0 0,64-12-1198,-68 13 914,34-4-6546</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1461.13">1694 84 24575,'0'4'0,"0"7"0,4 5 0,7 5 0,5 3 0,0 2 0,-2 1 0,-4 1 0,1-1 0,-2 1 0,-1-6-8191</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14452BDB-EEF1-4AAB-A804-24BE778FF02A}">
   <dimension ref="B2:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +1020,7 @@
       <c r="O2" s="1">
         <v>58</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -520,7 +1055,7 @@
       <c r="O3" s="1">
         <v>9</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="1">
         <f>INT((F3+O3)/2)</f>
         <v>4</v>
       </c>
@@ -556,10 +1091,10 @@
       <c r="P5" s="1">
         <v>58</v>
       </c>
-      <c r="T5" t="s">
-        <v>1</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="T5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -576,7 +1111,7 @@
       <c r="G6" s="1">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="1">
         <v>4</v>
       </c>
       <c r="L6" s="1">
@@ -594,11 +1129,11 @@
       <c r="P6" s="1">
         <v>9</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="1">
         <f>INT((D6+H6)/2)</f>
         <v>2</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="1">
         <f>INT((L6+P6)/2)</f>
         <v>7</v>
       </c>
@@ -634,16 +1169,16 @@
       <c r="P8" s="1">
         <v>58</v>
       </c>
-      <c r="T8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
+      <c r="T8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -654,13 +1189,13 @@
       <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="G9" s="2">
         <v>3</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="1">
         <v>4</v>
       </c>
       <c r="K9" s="1">
@@ -669,7 +1204,7 @@
       <c r="L9" s="2">
         <v>6</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="1">
         <v>7</v>
       </c>
       <c r="O9" s="2">
@@ -678,19 +1213,19 @@
       <c r="P9" s="1">
         <v>9</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="1">
         <f>INT((C9+E9)/2)</f>
         <v>1</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="1">
         <f>INT((G9+H9)/2)</f>
         <v>3</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="1">
         <f>INT((K9+M9)/2)</f>
         <v>6</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="1">
         <f>INT((O9+P9)/2)</f>
         <v>8</v>
       </c>
@@ -726,10 +1261,10 @@
       <c r="R11" s="1">
         <v>58</v>
       </c>
-      <c r="T11" t="s">
-        <v>1</v>
-      </c>
-      <c r="U11" t="s">
+      <c r="T11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -740,13 +1275,13 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <v>3</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="1">
         <v>4</v>
       </c>
       <c r="K12" s="1">
@@ -755,20 +1290,20 @@
       <c r="L12" s="2">
         <v>6</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="1">
         <v>7</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="3">
         <v>8</v>
       </c>
       <c r="R12" s="1">
         <v>9</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="1">
         <f>B12+C12</f>
         <v>1</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="1">
         <f>INT((K12+L12)/2)</f>
         <v>5</v>
       </c>
@@ -782,14 +1317,538 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="K15" s="3">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379B843-8543-4382-BA37-E388C22FD75F}">
+  <dimension ref="B2:W23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1">
+        <v>87</v>
+      </c>
+      <c r="J2" s="1">
+        <v>81</v>
+      </c>
+      <c r="K2" s="1">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1">
+        <v>99</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1">
+        <v>58</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <v>7</v>
+      </c>
+      <c r="N3" s="1">
+        <v>8</v>
+      </c>
+      <c r="O3" s="1">
+        <v>9</v>
+      </c>
+      <c r="T3" s="1">
+        <f>INT((F3+O3)/2)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>74</v>
+      </c>
+      <c r="F5" s="1">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1">
+        <v>81</v>
+      </c>
+      <c r="H5" s="1">
+        <v>81</v>
+      </c>
+      <c r="L5" s="1">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1">
+        <v>25</v>
+      </c>
+      <c r="N5" s="1">
+        <v>99</v>
+      </c>
+      <c r="O5" s="1">
+        <v>44</v>
+      </c>
+      <c r="P5" s="1">
+        <v>58</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6</v>
+      </c>
+      <c r="N6" s="2">
+        <v>7</v>
+      </c>
+      <c r="O6" s="1">
+        <v>8</v>
+      </c>
+      <c r="P6" s="1">
+        <v>9</v>
+      </c>
+      <c r="T6" s="1">
+        <f>INT((D6+H6)/2)</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="1">
+        <f>INT((L6+P6)/2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1">
+        <v>74</v>
+      </c>
+      <c r="G8" s="1">
+        <v>81</v>
+      </c>
+      <c r="H8" s="1">
+        <v>87</v>
+      </c>
+      <c r="K8" s="1">
+        <v>16</v>
+      </c>
+      <c r="L8" s="1">
+        <v>25</v>
+      </c>
+      <c r="M8" s="1">
+        <v>99</v>
+      </c>
+      <c r="O8" s="1">
+        <v>44</v>
+      </c>
+      <c r="P8" s="1">
+        <v>58</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
+      <c r="L9" s="2">
+        <v>6</v>
+      </c>
+      <c r="M9" s="1">
+        <v>7</v>
+      </c>
+      <c r="O9" s="2">
+        <v>8</v>
+      </c>
+      <c r="P9" s="1">
+        <v>9</v>
+      </c>
+      <c r="T9" s="1">
+        <f>INT((C9+E9)/2)</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="1">
+        <f>INT((G9+H9)/2)</f>
+        <v>3</v>
+      </c>
+      <c r="V9" s="1">
+        <f>INT((K9+M9)/2)</f>
+        <v>6</v>
+      </c>
+      <c r="W9" s="1">
+        <f>INT((O9+P9)/2)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1">
+        <v>74</v>
+      </c>
+      <c r="G11" s="1">
+        <v>87</v>
+      </c>
+      <c r="I11" s="1">
+        <v>81</v>
+      </c>
+      <c r="K11" s="1">
+        <v>16</v>
+      </c>
+      <c r="L11" s="1">
+        <v>25</v>
+      </c>
+      <c r="N11" s="1">
+        <v>99</v>
+      </c>
+      <c r="P11" s="1">
+        <v>44</v>
+      </c>
+      <c r="R11" s="1">
+        <v>58</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
+      <c r="L12" s="2">
+        <v>6</v>
+      </c>
+      <c r="N12" s="1">
+        <v>7</v>
+      </c>
+      <c r="P12" s="3">
+        <v>8</v>
+      </c>
+      <c r="R12" s="1">
+        <v>9</v>
+      </c>
+      <c r="T12" s="1">
+        <f>B12+C12</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="1">
+        <f>INT((K12+L12)/2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1">
+        <v>87</v>
+      </c>
+      <c r="F18" s="1">
+        <v>81</v>
+      </c>
+      <c r="G18" s="1">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1">
+        <v>99</v>
+      </c>
+      <c r="J18" s="1">
+        <v>44</v>
+      </c>
+      <c r="K18" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1">
+        <v>6</v>
+      </c>
+      <c r="I19" s="1">
+        <v>7</v>
+      </c>
+      <c r="J19" s="1">
+        <v>8</v>
+      </c>
+      <c r="K19" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>74</v>
+      </c>
+      <c r="C22" s="1">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1">
+        <v>7</v>
+      </c>
+      <c r="J23" s="1">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="B21:K21"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>